<commit_message>
Competing ahora funcional (quedan las otras variables)
</commit_message>
<xml_diff>
--- a/Competing_descompensacio.xlsx
+++ b/Competing_descompensacio.xlsx
@@ -448,7 +448,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -708,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14">
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -812,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
@@ -1020,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1098,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>126.8</v>
       </c>
     </row>
     <row r="34">
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -1592,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48">
@@ -1618,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
@@ -1644,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -1748,7 +1748,7 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54">
@@ -1852,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58">
@@ -1930,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61">
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68">
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70">
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72">
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -2684,7 +2684,7 @@
         <v>1</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90">
@@ -2736,7 +2736,7 @@
         <v>1</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="92">
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102">
@@ -3074,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105">
@@ -3100,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106">
@@ -3334,7 +3334,7 @@
         <v>1</v>
       </c>
       <c r="H114">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115">
@@ -3464,7 +3464,7 @@
         <v>1</v>
       </c>
       <c r="H119">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120">
@@ -3672,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="H127">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="128">
@@ -3828,7 +3828,7 @@
         <v>1</v>
       </c>
       <c r="H133">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="134">
@@ -4166,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="H146">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="147">
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
       <c r="H149">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150">
@@ -4348,7 +4348,7 @@
         <v>1</v>
       </c>
       <c r="H153">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="154">
@@ -4400,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="H155">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156">
@@ -4426,7 +4426,7 @@
         <v>1</v>
       </c>
       <c r="H156">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="157">
@@ -4530,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="H160">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="161">
@@ -4686,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="H166">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167">
@@ -4712,7 +4712,7 @@
         <v>1</v>
       </c>
       <c r="H167">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168">
@@ -4842,7 +4842,7 @@
         <v>1</v>
       </c>
       <c r="H172">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="173">
@@ -4972,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="H177">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -4998,7 +4998,7 @@
         <v>1</v>
       </c>
       <c r="H178">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="179">
@@ -5050,7 +5050,7 @@
         <v>1</v>
       </c>
       <c r="H180">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181">
@@ -5388,7 +5388,7 @@
         <v>1</v>
       </c>
       <c r="H193">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="194">
@@ -5544,7 +5544,7 @@
         <v>1</v>
       </c>
       <c r="H199">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -6090,7 +6090,7 @@
         <v>1</v>
       </c>
       <c r="H220">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221">
@@ -6220,7 +6220,7 @@
         <v>1</v>
       </c>
       <c r="H225">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="226">
@@ -6324,7 +6324,7 @@
         <v>1</v>
       </c>
       <c r="H229">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="230">
@@ -6376,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="H231">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="232">
@@ -6402,7 +6402,7 @@
         <v>1</v>
       </c>
       <c r="H232">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233">
@@ -6506,7 +6506,7 @@
         <v>1</v>
       </c>
       <c r="H236">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -6610,7 +6610,7 @@
         <v>1</v>
       </c>
       <c r="H240">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="241">
@@ -6766,7 +6766,7 @@
         <v>1</v>
       </c>
       <c r="H246">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">
@@ -6867,10 +6867,10 @@
         <v>1</v>
       </c>
       <c r="G250">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H250">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
@@ -7364,7 +7364,7 @@
         <v>1</v>
       </c>
       <c r="H269">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">
@@ -7780,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="H285">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286">
@@ -7832,7 +7832,7 @@
         <v>1</v>
       </c>
       <c r="H287">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288">
@@ -7910,7 +7910,7 @@
         <v>1</v>
       </c>
       <c r="H290">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="291">
@@ -8375,10 +8375,10 @@
         <v>31</v>
       </c>
       <c r="G308">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H308">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="309">
@@ -8638,7 +8638,7 @@
         <v>1</v>
       </c>
       <c r="H318">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319">
@@ -8664,7 +8664,7 @@
         <v>1</v>
       </c>
       <c r="H319">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="320">
@@ -8742,7 +8742,7 @@
         <v>1</v>
       </c>
       <c r="H322">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323">
@@ -8898,7 +8898,7 @@
         <v>1</v>
       </c>
       <c r="H328">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329">
@@ -8924,7 +8924,7 @@
         <v>1</v>
       </c>
       <c r="H329">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="330">
@@ -9106,7 +9106,7 @@
         <v>1</v>
       </c>
       <c r="H336">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="337">
@@ -9262,7 +9262,7 @@
         <v>1</v>
       </c>
       <c r="H342">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="343">
@@ -9574,7 +9574,7 @@
         <v>1</v>
       </c>
       <c r="H354">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355">
@@ -9756,7 +9756,7 @@
         <v>1</v>
       </c>
       <c r="H361">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362">
@@ -9834,7 +9834,7 @@
         <v>1</v>
       </c>
       <c r="H364">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365">
@@ -10016,7 +10016,7 @@
         <v>1</v>
       </c>
       <c r="H371">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="372">
@@ -10042,7 +10042,7 @@
         <v>1</v>
       </c>
       <c r="H372">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>